<commit_message>
combine normal and negative test case
</commit_message>
<xml_diff>
--- a/acc whistle.xlsx
+++ b/acc whistle.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\git\acc_whistle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test data login" sheetId="4" r:id="rId1"/>
-    <sheet name="test data daftar" sheetId="2" r:id="rId2"/>
-    <sheet name="test data search tiket" sheetId="3" r:id="rId3"/>
+    <sheet name="test data search tiket" sheetId="5" r:id="rId2"/>
+    <sheet name="test data daftar" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>email</t>
   </si>
@@ -103,12 +103,6 @@
     <t>ch24006007</t>
   </si>
   <si>
-    <t>ch24006118</t>
-  </si>
-  <si>
-    <t>ch24006119</t>
-  </si>
-  <si>
     <t>no_tiket</t>
   </si>
   <si>
@@ -119,13 +113,34 @@
   </si>
   <si>
     <t>PLP20190823003</t>
+  </si>
+  <si>
+    <t>PLP 20190823001</t>
+  </si>
+  <si>
+    <t>PLP20190823004</t>
+  </si>
+  <si>
+    <t>terdaftar</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>input tidak terdaftar</t>
+  </si>
+  <si>
+    <t>input kosong</t>
+  </si>
+  <si>
+    <t>input dengan spasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +170,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -165,7 +187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -225,19 +247,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="C1" sqref="C1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,56 +555,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -699,74 +797,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add login check revision
</commit_message>
<xml_diff>
--- a/acc whistle.xlsx
+++ b/acc whistle.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="test data login" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>email</t>
   </si>
@@ -134,6 +134,30 @@
   </si>
   <si>
     <t>input dengan spasi</t>
+  </si>
+  <si>
+    <t>christianti.angelin@tiukdwacid</t>
+  </si>
+  <si>
+    <t>email tidak sesuai format</t>
+  </si>
+  <si>
+    <t>email &amp; paswword kosong</t>
+  </si>
+  <si>
+    <t>email kosong</t>
+  </si>
+  <si>
+    <t>password kosong</t>
+  </si>
+  <si>
+    <t>password salah</t>
+  </si>
+  <si>
+    <t>email salah</t>
+  </si>
+  <si>
+    <t>berhasil login</t>
   </si>
 </sst>
 </file>
@@ -220,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -254,6 +278,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,64 +567,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="12"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>3</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -608,6 +666,7 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -617,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>